<commit_message>
tentative fix to key error
</commit_message>
<xml_diff>
--- a/empty_dataset.xlsx
+++ b/empty_dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nsg/PycharmProjects/MockData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C27E0B-CFAD-4D4D-B1B6-9A75EBF5C441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C363B2-EC0B-BA47-AA7B-7E441FDE46ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="21380" windowHeight="19820" xr2:uid="{82BC8D1E-D205-7442-9BAC-CB2917E1B727}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
   <si>
     <t>Patient_ID</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>Categorical</t>
-  </si>
-  <si>
-    <t>10, 5</t>
   </si>
 </sst>
 </file>
@@ -586,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A51439-064E-414C-8393-BDCA0965CEC3}">
-  <dimension ref="A1:AX3"/>
+  <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -898,14 +895,6 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3">
-        <v>55</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>